<commit_message>
Updated Procedure to 8-7-2025 XtEHR version
</commit_message>
<xml_diff>
--- a/maps/Procedure.xlsx
+++ b/maps/Procedure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\mgraauw\eu-nl-compared\maps\xtehr2zibs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Nictiz\eu-nl-compared\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F59B1A-4512-473D-8401-B09144555A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FC47B4-99C5-4D57-8BC8-E37FA4C7BBD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4155" yWindow="-18000" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
   <si>
     <t>EHDSProcedure</t>
   </si>
   <si>
-    <t>EHDSProcedure.identifier</t>
-  </si>
-  <si>
-    <t>EHDSProcedure.description</t>
-  </si>
-  <si>
     <t>EHDSProcedure.code</t>
   </si>
   <si>
@@ -40,12 +34,6 @@
     <t>EHDSProcedure.performer</t>
   </si>
   <si>
-    <t>EHDSProcedure.anatomicLocation</t>
-  </si>
-  <si>
-    <t>EHDSProcedure.reason</t>
-  </si>
-  <si>
     <t>EHDSProcedure.outcome</t>
   </si>
   <si>
@@ -64,9 +52,6 @@
     <t>EHDSProcedure.note</t>
   </si>
   <si>
-    <t>EHDSProcedure.subject</t>
-  </si>
-  <si>
     <t>xtehr</t>
   </si>
   <si>
@@ -119,6 +104,51 @@
   </si>
   <si>
     <t>Procedure.Indication.Symptom</t>
+  </si>
+  <si>
+    <t>EHDSProcedure.header</t>
+  </si>
+  <si>
+    <t>EHDSProcedure.presentedForm</t>
+  </si>
+  <si>
+    <t>EHDSProcedure.bodySite</t>
+  </si>
+  <si>
+    <t>EHDSProcedure.reason[x]</t>
+  </si>
+  <si>
+    <t>Registratiegegevens, zie DataSet mapping</t>
+  </si>
+  <si>
+    <t>EHDSProcedure.header.subject</t>
+  </si>
+  <si>
+    <t>EHDSProcedure.header.identifier</t>
+  </si>
+  <si>
+    <t>EHDSProcedure.header.authorship</t>
+  </si>
+  <si>
+    <t>EHDSProcedure.header.authorship.author[x]</t>
+  </si>
+  <si>
+    <t>EHDSProcedure.header.authorship.datetime</t>
+  </si>
+  <si>
+    <t>EHDSProcedure.header.lastUpdate</t>
+  </si>
+  <si>
+    <t>EHDSProcedure.header.status</t>
+  </si>
+  <si>
+    <t>EHDSProcedure.header.statusReason[x]</t>
+  </si>
+  <si>
+    <t>EHDSProcedure.header.language</t>
+  </si>
+  <si>
+    <t>EHDSProcedure.header.version</t>
   </si>
 </sst>
 </file>
@@ -481,24 +511,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C1">
         <v>2020</v>
@@ -512,220 +542,268 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
+      <c r="A9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>14</v>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>7</v>
       </c>
-      <c r="B23" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" t="s">
-        <v>28</v>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>